<commit_message>
added support for groups of size 5
</commit_message>
<xml_diff>
--- a/peer_eval/grade_matrix.xlsx
+++ b/peer_eval/grade_matrix.xlsx
@@ -1,18 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nate/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="19020" yWindow="10920" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="M2" sheetId="1" r:id="rId1"/>
-    <sheet name="M3" sheetId="2" r:id="rId2"/>
-    <sheet name="M4" sheetId="3" r:id="rId3"/>
+    <sheet name="Params" sheetId="4" r:id="rId1"/>
+    <sheet name="M2" sheetId="1" r:id="rId2"/>
+    <sheet name="M3" sheetId="2" r:id="rId3"/>
+    <sheet name="M4" sheetId="3" r:id="rId4"/>
+    <sheet name="M5" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -21,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="8">
   <si>
     <t>M1</t>
   </si>
@@ -42,6 +52,9 @@
   </si>
   <si>
     <t>Individual Grades</t>
+  </si>
+  <si>
+    <t>M5</t>
   </si>
 </sst>
 </file>
@@ -90,8 +103,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -116,7 +133,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -127,6 +144,8 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -137,10 +156,17 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -466,19 +492,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -489,10 +538,11 @@
         <v>5</v>
       </c>
       <c r="F1">
+        <f>Params!B1</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -503,12 +553,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4">
         <f>SUM(B2:B3)</f>
         <v>0</v>
@@ -518,7 +568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="e">
         <f>B4/SUM(B4:C4)</f>
         <v>#DIV/0!</v>
@@ -528,7 +578,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -544,29 +594,24 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -580,10 +625,11 @@
         <v>5</v>
       </c>
       <c r="G1">
+        <f>Params!B1</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -594,17 +640,17 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5">
         <f>SUM(B2:B4)</f>
         <v>0</v>
@@ -618,7 +664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="e">
         <f>B5/SUM(B5:D5)</f>
         <v>#DIV/0!</v>
@@ -632,7 +678,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -652,29 +698,24 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -691,10 +732,11 @@
         <v>5</v>
       </c>
       <c r="H1">
+        <f>Params!B1</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -705,22 +747,40 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <f>SUM(B2:B5)</f>
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="0">SUM(C2:C5)</f>
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" t="e">
         <f>B6/SUM(B6:E6)</f>
         <v>#DIV/0!</v>
@@ -738,7 +798,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -747,25 +807,164 @@
         <v>#DIV/0!</v>
       </c>
       <c r="C10" t="e">
-        <f t="shared" ref="C10:E10" si="0">($H$1*$H$2*C7*4)+($H$2*(1-$H$1))</f>
+        <f t="shared" ref="C10:E10" si="1">($H$1*$H$2*C7*4)+($H$2*(1-$H$1))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D10" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="E10" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1">
+        <f>Params!B1</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <f>SUM(B2:B6)</f>
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:F7" si="0">SUM(C2:C6)</f>
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B8" t="e">
+        <f>B7/SUM($B7:$F7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C8" t="e">
+        <f t="shared" ref="C8:F8" si="1">C7/SUM($B7:$F7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F8" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="e">
+        <f>($I$1*$I$2*B8*5)+($I$2*(1-$I$1))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C11" t="e">
+        <f t="shared" ref="C11:F11" si="2">($I$1*$I$2*C8*5)+($I$2*(1-$I$1))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D11" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E11" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F11" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
by default, columns labels copy rows
</commit_message>
<xml_diff>
--- a/peer_eval/grade_matrix.xlsx
+++ b/peer_eval/grade_matrix.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nate/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nate/Documents/repos/neu-templates/peer_eval/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19020" yWindow="10920" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="1260" yWindow="1720" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Params" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="8">
   <si>
     <t>M1</t>
   </si>
@@ -518,7 +518,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,11 +528,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
+      <c r="B1" t="str">
+        <f>A2</f>
+        <v>M1</v>
+      </c>
+      <c r="C1" t="str">
+        <f>A3</f>
+        <v>M2</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
@@ -602,7 +604,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,14 +614,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
+      <c r="B1" t="str">
+        <f>A2</f>
+        <v>M1</v>
+      </c>
+      <c r="C1" t="str">
+        <f>A3</f>
+        <v>M2</v>
+      </c>
+      <c r="D1" t="str">
+        <f>A4</f>
+        <v>M3</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -706,7 +711,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -716,17 +721,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
+      <c r="B1" t="str">
+        <f>A2</f>
+        <v>M1</v>
+      </c>
+      <c r="C1" t="str">
+        <f>A3</f>
+        <v>M2</v>
+      </c>
+      <c r="D1" t="str">
+        <f>A4</f>
+        <v>M3</v>
+      </c>
+      <c r="E1" t="str">
+        <f>A5</f>
+        <v>M4</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -830,7 +839,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -840,20 +849,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
+      <c r="B1" t="str">
+        <f>A2</f>
+        <v>M1</v>
+      </c>
+      <c r="C1" t="str">
+        <f>A3</f>
+        <v>M2</v>
+      </c>
+      <c r="D1" t="str">
+        <f>A4</f>
+        <v>M3</v>
+      </c>
+      <c r="E1" t="str">
+        <f>A5</f>
+        <v>M4</v>
+      </c>
+      <c r="F1" t="str">
+        <f>A6</f>
+        <v>M5</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>

</xml_diff>